<commit_message>
feat: redesigned project emx
</commit_message>
<xml_diff>
--- a/model/organisations.xlsx
+++ b/model/organisations.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidcruvolo/Github/projects-rd-dashboards/model/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E774504E-9825-8C46-BD40-45678F2FFE23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9B9E139-80FE-1A44-83E4-1D16F3ACBAF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-29720" yWindow="-1760" windowWidth="19220" windowHeight="17720" activeTab="2" xr2:uid="{BF6F49B7-B9CF-3840-9FDA-0A48BFD82D3F}"/>
+    <workbookView xWindow="-38400" yWindow="-3180" windowWidth="38400" windowHeight="21100" activeTab="2" xr2:uid="{BF6F49B7-B9CF-3840-9FDA-0A48BFD82D3F}"/>
   </bookViews>
   <sheets>
     <sheet name="packages" sheetId="1" r:id="rId1"/>
     <sheet name="entities" sheetId="2" r:id="rId2"/>
     <sheet name="attributes" sheetId="3" r:id="rId3"/>
+    <sheet name="tags" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="91">
   <si>
     <t>name</t>
   </si>
@@ -79,18 +80,9 @@
     <t>code</t>
   </si>
   <si>
-    <t>projectOfficialName</t>
-  </si>
-  <si>
-    <t>department</t>
-  </si>
-  <si>
     <t>aliases</t>
   </si>
   <si>
-    <t>alternativeIdentifiers</t>
-  </si>
-  <si>
     <t>country</t>
   </si>
   <si>
@@ -118,15 +110,9 @@
     <t>package</t>
   </si>
   <si>
-    <t>iri</t>
-  </si>
-  <si>
     <t>hyperlink</t>
   </si>
   <si>
-    <t>variations</t>
-  </si>
-  <si>
     <t>Variations</t>
   </si>
   <si>
@@ -139,44 +125,211 @@
     <t>refEntity</t>
   </si>
   <si>
-    <t>organisations_variations</t>
-  </si>
-  <si>
     <t>organisation</t>
   </si>
   <si>
-    <t>variation</t>
-  </si>
-  <si>
-    <t>children</t>
-  </si>
-  <si>
-    <t>Child Relationships</t>
-  </si>
-  <si>
     <t>Name variations of organisations</t>
   </si>
   <si>
-    <t>Child affiliations associated with the organisation (e.g., department, institute, etc.)</t>
-  </si>
-  <si>
-    <t>organisations_children</t>
-  </si>
-  <si>
     <t>labelAttribute</t>
   </si>
   <si>
     <t>lookupAttribute</t>
+  </si>
+  <si>
+    <t>A textual identifier for an organization.</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C93874</t>
+  </si>
+  <si>
+    <t>The unique identification of an organization in a specified context.</t>
+  </si>
+  <si>
+    <t>NCIT:C93401</t>
+  </si>
+  <si>
+    <t>NCIT:C93874</t>
+  </si>
+  <si>
+    <t>A specialized division of a large organization.</t>
+  </si>
+  <si>
+    <t>NCIT:C42671</t>
+  </si>
+  <si>
+    <t>NCIT:C20108</t>
+  </si>
+  <si>
+    <t>An alphanumeric system designed to identify countries. The ISO 3166 standard includes a two letter representation, a three letter representation, and a 3 number representation. The last two are identical to the UN system. The US State Department system maintains a separate two letter representation code set.</t>
+  </si>
+  <si>
+    <t>NCIT:C25464</t>
+  </si>
+  <si>
+    <t>A collective generic term that refers here to a wide variety of dependencies, areas of special sovereignty, uninhabited islands, and other entities in addition to the traditional countries or independent states.</t>
+  </si>
+  <si>
+    <t>NCIT:C25160</t>
+  </si>
+  <si>
+    <t>A large and densely populated urban area; a city specified in an address.</t>
+  </si>
+  <si>
+    <t>NCIT:C68642</t>
+  </si>
+  <si>
+    <t>The angular distance north or south between an imaginary line around a heavenly body parallel to its equator and the equator itself.</t>
+  </si>
+  <si>
+    <t>NCIT:C68643</t>
+  </si>
+  <si>
+    <t>An imaginary great circle on the surface of a heavenly body passing through the poles at right angles to the equator.</t>
+  </si>
+  <si>
+    <t>project</t>
+  </si>
+  <si>
+    <t>organisations_namevariations</t>
+  </si>
+  <si>
+    <t>organisations_suborganisations</t>
+  </si>
+  <si>
+    <t>identifier</t>
+  </si>
+  <si>
+    <t>NCIT:C25364</t>
+  </si>
+  <si>
+    <t>One or more characters used to identify, name, or characterize the nature, properties, or contents of a thing.</t>
+  </si>
+  <si>
+    <t>mref</t>
+  </si>
+  <si>
+    <t>NCIT:C165056</t>
+  </si>
+  <si>
+    <t>The name applied to an investigational project.</t>
+  </si>
+  <si>
+    <t>NCIT:C42778</t>
+  </si>
+  <si>
+    <t>A string of characters used to identify or name a resource on the Internet. Such identification enables interaction with representations of the resource over a network, typically the World Wide Web, using specific protocols. MIT data management and publishing</t>
+  </si>
+  <si>
+    <t>uri</t>
+  </si>
+  <si>
+    <t>objectIRI</t>
+  </si>
+  <si>
+    <t>codeSystem</t>
+  </si>
+  <si>
+    <t>relationLabel</t>
+  </si>
+  <si>
+    <t>relationIRI</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C93401</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C42778</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C25464</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C20108</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C25160</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C68642</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C68643</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C42671</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C25364</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C165056</t>
+  </si>
+  <si>
+    <t>NCIT</t>
+  </si>
+  <si>
+    <t>isAssociatedWith</t>
+  </si>
+  <si>
+    <t>http://molgenis.org#isAssociatedWith</t>
+  </si>
+  <si>
+    <t>projects</t>
+  </si>
+  <si>
+    <t>namevariations</t>
+  </si>
+  <si>
+    <t>suborganisations</t>
+  </si>
+  <si>
+    <t>Child entities associated with the organisation (e.g., department, institute, etc.)</t>
+  </si>
+  <si>
+    <t>Projects</t>
+  </si>
+  <si>
+    <t>Sub Organisations</t>
+  </si>
+  <si>
+    <t>Project organisation links</t>
+  </si>
+  <si>
+    <t>tags</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/GSSO_007214</t>
+  </si>
+  <si>
+    <t>GSSO:007214</t>
+  </si>
+  <si>
+    <t>GSSO</t>
+  </si>
+  <si>
+    <t>A name that a person or group assumes for a particular purpose, which can differ from their first or true name (orthonym).</t>
+  </si>
+  <si>
+    <t>organisations_projects</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -199,13 +352,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -559,15 +715,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20D2CF89-6078-A549-BBA8-9CDB1C9E7895}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.33203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="70.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
@@ -584,7 +740,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -603,13 +759,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>79</v>
       </c>
       <c r="B3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" t="s">
         <v>29</v>
-      </c>
-      <c r="C3" t="s">
-        <v>38</v>
       </c>
       <c r="D3" t="s">
         <v>3</v>
@@ -617,15 +773,29 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>36</v>
+        <v>80</v>
       </c>
       <c r="B4" t="s">
-        <v>37</v>
+        <v>83</v>
       </c>
       <c r="C4" t="s">
-        <v>39</v>
+        <v>81</v>
       </c>
       <c r="D4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D5" t="s">
         <v>3</v>
       </c>
     </row>
@@ -636,19 +806,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF4DB9BC-7108-9048-9421-519F0A2603E5}">
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="24.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -665,18 +836,24 @@
         <v>10</v>
       </c>
       <c r="F1" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="G1" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="H1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+      <c r="I1" t="s">
+        <v>85</v>
+      </c>
+      <c r="J1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B2" t="s">
         <v>12</v>
@@ -690,21 +867,33 @@
       <c r="E2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I2" t="s">
+        <v>35</v>
+      </c>
+      <c r="J2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I3" t="s">
+        <v>58</v>
+      </c>
+      <c r="J3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>26</v>
-      </c>
-      <c r="C3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>31</v>
       </c>
       <c r="B4" t="s">
         <v>0</v>
@@ -718,10 +907,16 @@
       <c r="H4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I4" t="s">
+        <v>36</v>
+      </c>
+      <c r="J4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B5" t="s">
         <v>13</v>
@@ -729,32 +924,50 @@
       <c r="C5" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I5" t="s">
+        <v>87</v>
+      </c>
+      <c r="J5" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C6" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I6" t="s">
+        <v>41</v>
+      </c>
+      <c r="J6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C7" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I7" t="s">
+        <v>39</v>
+      </c>
+      <c r="J7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B8" t="s">
         <v>16</v>
@@ -762,79 +975,107 @@
       <c r="C8" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I8" t="s">
+        <v>43</v>
+      </c>
+      <c r="J8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B9" t="s">
         <v>17</v>
       </c>
       <c r="C9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+      <c r="I9" t="s">
+        <v>45</v>
+      </c>
+      <c r="J9" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B10" t="s">
         <v>18</v>
       </c>
       <c r="C10" t="s">
+        <v>19</v>
+      </c>
+      <c r="I10" t="s">
+        <v>47</v>
+      </c>
+      <c r="J10" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>50</v>
+      </c>
+      <c r="B13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>31</v>
-      </c>
-      <c r="B11" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>31</v>
-      </c>
-      <c r="B12" t="s">
-        <v>20</v>
-      </c>
-      <c r="C12" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>31</v>
-      </c>
-      <c r="B13" t="s">
-        <v>21</v>
-      </c>
-      <c r="C13" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E13" t="b">
+        <v>0</v>
+      </c>
+      <c r="I13" t="s">
+        <v>36</v>
+      </c>
+      <c r="J13" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>31</v>
+        <v>50</v>
       </c>
       <c r="B14" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="C14" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+      <c r="F14" t="s">
+        <v>26</v>
+      </c>
+      <c r="I14" t="s">
+        <v>35</v>
+      </c>
+      <c r="J14" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>33</v>
+        <v>51</v>
       </c>
       <c r="B16" t="s">
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="C16" t="s">
         <v>11</v>
@@ -845,53 +1086,427 @@
       <c r="E16" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="I16" t="s">
+        <v>38</v>
+      </c>
+      <c r="J16" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>33</v>
+        <v>51</v>
       </c>
       <c r="B17" t="s">
+        <v>52</v>
+      </c>
+      <c r="C17" t="s">
+        <v>11</v>
+      </c>
+      <c r="I17" t="s">
+        <v>53</v>
+      </c>
+      <c r="J17" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>51</v>
+      </c>
+      <c r="B18" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" t="s">
+        <v>25</v>
+      </c>
+      <c r="F18" t="s">
+        <v>26</v>
+      </c>
+      <c r="I18" t="s">
+        <v>35</v>
+      </c>
+      <c r="J18" t="s">
         <v>34</v>
       </c>
-      <c r="C17" t="s">
-        <v>30</v>
-      </c>
-      <c r="F17" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>40</v>
-      </c>
-      <c r="B19" t="s">
-        <v>14</v>
-      </c>
-      <c r="C19" t="s">
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>90</v>
+      </c>
+      <c r="B20" t="s">
+        <v>0</v>
+      </c>
+      <c r="C20" t="s">
         <v>11</v>
       </c>
-      <c r="D19" t="b">
+      <c r="D20" t="b">
         <v>1</v>
       </c>
-      <c r="E19" t="b">
+      <c r="E20" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>40</v>
-      </c>
-      <c r="B20" t="s">
+      <c r="I20" t="s">
+        <v>36</v>
+      </c>
+      <c r="J20" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>90</v>
+      </c>
+      <c r="B21" t="s">
+        <v>52</v>
+      </c>
+      <c r="C21" t="s">
+        <v>11</v>
+      </c>
+      <c r="I21" t="s">
+        <v>53</v>
+      </c>
+      <c r="J21" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>90</v>
+      </c>
+      <c r="B22" t="s">
+        <v>49</v>
+      </c>
+      <c r="C22" t="s">
+        <v>11</v>
+      </c>
+      <c r="I22" t="s">
+        <v>56</v>
+      </c>
+      <c r="J22" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>90</v>
+      </c>
+      <c r="B23" t="s">
+        <v>28</v>
+      </c>
+      <c r="C23" t="s">
+        <v>55</v>
+      </c>
+      <c r="F23" t="s">
+        <v>26</v>
+      </c>
+      <c r="I23" t="s">
+        <v>35</v>
+      </c>
+      <c r="J23" t="s">
         <v>34</v>
-      </c>
-      <c r="C20" t="s">
-        <v>30</v>
-      </c>
-      <c r="F20" t="s">
-        <v>31</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65581772-3758-1740-81CA-91C7E8965EDD}">
+  <dimension ref="A1:F13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="33.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E2" t="s">
+        <v>76</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E3" t="s">
+        <v>76</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D4" t="s">
+        <v>75</v>
+      </c>
+      <c r="E4" t="s">
+        <v>76</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C5" t="s">
+        <v>73</v>
+      </c>
+      <c r="D5" t="s">
+        <v>75</v>
+      </c>
+      <c r="E5" t="s">
+        <v>76</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" t="s">
+        <v>72</v>
+      </c>
+      <c r="D6" t="s">
+        <v>75</v>
+      </c>
+      <c r="E6" t="s">
+        <v>76</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B7" t="s">
+        <v>58</v>
+      </c>
+      <c r="C7" t="s">
+        <v>66</v>
+      </c>
+      <c r="D7" t="s">
+        <v>75</v>
+      </c>
+      <c r="E7" t="s">
+        <v>76</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E8" t="s">
+        <v>76</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B9" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" t="s">
+        <v>71</v>
+      </c>
+      <c r="D9" t="s">
+        <v>75</v>
+      </c>
+      <c r="E9" t="s">
+        <v>76</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" t="s">
+        <v>65</v>
+      </c>
+      <c r="D10" t="s">
+        <v>75</v>
+      </c>
+      <c r="E10" t="s">
+        <v>76</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" t="s">
+        <v>75</v>
+      </c>
+      <c r="E11" t="s">
+        <v>76</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" t="s">
+        <v>67</v>
+      </c>
+      <c r="D12" t="s">
+        <v>75</v>
+      </c>
+      <c r="E12" t="s">
+        <v>76</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>87</v>
+      </c>
+      <c r="B13" t="s">
+        <v>87</v>
+      </c>
+      <c r="C13" t="s">
+        <v>86</v>
+      </c>
+      <c r="D13" t="s">
+        <v>88</v>
+      </c>
+      <c r="E13" t="s">
+        <v>76</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F11">
+    <sortCondition ref="A2:A11"/>
+  </sortState>
+  <hyperlinks>
+    <hyperlink ref="F2" r:id="rId1" location="isAssociatedWith" xr:uid="{9CAB4221-0840-AE47-B477-83A322DE3FF6}"/>
+    <hyperlink ref="F3" r:id="rId2" location="isAssociatedWith" xr:uid="{67740F16-9B9F-CB41-829C-97A2A4A077B6}"/>
+    <hyperlink ref="F4" r:id="rId3" location="isAssociatedWith" xr:uid="{03E0772E-F750-2542-90FD-38B880F280FB}"/>
+    <hyperlink ref="F5" r:id="rId4" location="isAssociatedWith" xr:uid="{33698B68-797A-5642-BC4E-7E7C2E97C462}"/>
+    <hyperlink ref="F6" r:id="rId5" location="isAssociatedWith" xr:uid="{A500A2CD-D6AB-EC4F-B666-BCC7F5FFB5E3}"/>
+    <hyperlink ref="F7" r:id="rId6" location="isAssociatedWith" xr:uid="{294C7113-A988-F048-99F0-B004EB4D6380}"/>
+    <hyperlink ref="F8" r:id="rId7" location="isAssociatedWith" xr:uid="{8BB1E4A2-75D2-0C42-AF22-2D6DD795257C}"/>
+    <hyperlink ref="F9" r:id="rId8" location="isAssociatedWith" xr:uid="{A4E6A691-FB67-0241-9B8B-6A23D51842F0}"/>
+    <hyperlink ref="F10" r:id="rId9" location="isAssociatedWith" xr:uid="{28CABF14-DBF3-7040-B5D8-FDDFD45A12D4}"/>
+    <hyperlink ref="F11" r:id="rId10" location="isAssociatedWith" xr:uid="{FC3B23FF-ADCC-4640-BF09-FDDCDD30E681}"/>
+    <hyperlink ref="F12" r:id="rId11" location="isAssociatedWith" xr:uid="{29A26427-919D-8645-8906-F24950CBC0F1}"/>
+    <hyperlink ref="F13" r:id="rId12" location="isAssociatedWith" xr:uid="{5D48DF7B-6595-7741-86E3-8D917AE9E72F}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
fix: edits to model
</commit_message>
<xml_diff>
--- a/model/organisations.xlsx
+++ b/model/organisations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidcruvolo/Github/projects-rd-dashboards/model/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9B9E139-80FE-1A44-83E4-1D16F3ACBAF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63340094-29E9-7F4B-B270-7A422C8CDD29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38400" yWindow="-3180" windowWidth="38400" windowHeight="21100" activeTab="2" xr2:uid="{BF6F49B7-B9CF-3840-9FDA-0A48BFD82D3F}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="90">
   <si>
     <t>name</t>
   </si>
@@ -204,9 +204,6 @@
   </si>
   <si>
     <t>One or more characters used to identify, name, or characterize the nature, properties, or contents of a thing.</t>
-  </si>
-  <si>
-    <t>mref</t>
   </si>
   <si>
     <t>NCIT:C165056</t>
@@ -759,7 +756,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B3" t="s">
         <v>24</v>
@@ -773,13 +770,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C4" t="s">
         <v>80</v>
-      </c>
-      <c r="B4" t="s">
-        <v>83</v>
-      </c>
-      <c r="C4" t="s">
-        <v>81</v>
       </c>
       <c r="D4" t="s">
         <v>3</v>
@@ -787,13 +784,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D5" t="s">
         <v>3</v>
@@ -809,7 +806,7 @@
   <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -845,7 +842,7 @@
         <v>31</v>
       </c>
       <c r="I1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J1" t="s">
         <v>2</v>
@@ -879,16 +876,16 @@
         <v>26</v>
       </c>
       <c r="B3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C3" t="s">
         <v>23</v>
       </c>
       <c r="I3" t="s">
+        <v>57</v>
+      </c>
+      <c r="J3" t="s">
         <v>58</v>
-      </c>
-      <c r="J3" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
@@ -925,10 +922,10 @@
         <v>11</v>
       </c>
       <c r="I5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
@@ -1132,7 +1129,7 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B20" t="s">
         <v>0</v>
@@ -1155,7 +1152,7 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B21" t="s">
         <v>52</v>
@@ -1172,7 +1169,7 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B22" t="s">
         <v>49</v>
@@ -1181,21 +1178,21 @@
         <v>11</v>
       </c>
       <c r="I22" t="s">
+        <v>55</v>
+      </c>
+      <c r="J22" t="s">
         <v>56</v>
-      </c>
-      <c r="J22" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B23" t="s">
         <v>28</v>
       </c>
       <c r="C23" t="s">
-        <v>55</v>
+        <v>25</v>
       </c>
       <c r="F23" t="s">
         <v>26</v>
@@ -1237,36 +1234,36 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1" t="s">
         <v>61</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>62</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>63</v>
-      </c>
-      <c r="F1" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D2" t="s">
         <v>74</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>75</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" s="1" t="s">
         <v>76</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -1277,16 +1274,16 @@
         <v>39</v>
       </c>
       <c r="C3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D3" t="s">
+        <v>74</v>
+      </c>
+      <c r="E3" t="s">
         <v>75</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" s="1" t="s">
         <v>76</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -1297,16 +1294,16 @@
         <v>43</v>
       </c>
       <c r="C4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D4" t="s">
+        <v>74</v>
+      </c>
+      <c r="E4" t="s">
         <v>75</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" s="1" t="s">
         <v>76</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -1317,16 +1314,16 @@
         <v>53</v>
       </c>
       <c r="C5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D5" t="s">
+        <v>74</v>
+      </c>
+      <c r="E5" t="s">
         <v>75</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" s="1" t="s">
         <v>76</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -1337,36 +1334,36 @@
         <v>38</v>
       </c>
       <c r="C6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D6" t="s">
+        <v>74</v>
+      </c>
+      <c r="E6" t="s">
         <v>75</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" s="1" t="s">
         <v>76</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D7" t="s">
+        <v>74</v>
+      </c>
+      <c r="E7" t="s">
         <v>75</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" s="1" t="s">
         <v>76</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -1377,16 +1374,16 @@
         <v>45</v>
       </c>
       <c r="C8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D8" t="s">
+        <v>74</v>
+      </c>
+      <c r="E8" t="s">
         <v>75</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" s="1" t="s">
         <v>76</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -1397,16 +1394,16 @@
         <v>47</v>
       </c>
       <c r="C9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D9" t="s">
+        <v>74</v>
+      </c>
+      <c r="E9" t="s">
         <v>75</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" s="1" t="s">
         <v>76</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -1417,16 +1414,16 @@
         <v>35</v>
       </c>
       <c r="C10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D10" t="s">
+        <v>74</v>
+      </c>
+      <c r="E10" t="s">
         <v>75</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" s="1" t="s">
         <v>76</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -1440,13 +1437,13 @@
         <v>33</v>
       </c>
       <c r="D11" t="s">
+        <v>74</v>
+      </c>
+      <c r="E11" t="s">
         <v>75</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" s="1" t="s">
         <v>76</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
@@ -1457,36 +1454,36 @@
         <v>41</v>
       </c>
       <c r="C12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D12" t="s">
+        <v>74</v>
+      </c>
+      <c r="E12" t="s">
         <v>75</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" s="1" t="s">
         <v>76</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>86</v>
+      </c>
+      <c r="B13" t="s">
+        <v>86</v>
+      </c>
+      <c r="C13" t="s">
+        <v>85</v>
+      </c>
+      <c r="D13" t="s">
         <v>87</v>
       </c>
-      <c r="B13" t="s">
-        <v>87</v>
-      </c>
-      <c r="C13" t="s">
-        <v>86</v>
-      </c>
-      <c r="D13" t="s">
-        <v>88</v>
-      </c>
       <c r="E13" t="s">
+        <v>75</v>
+      </c>
+      <c r="F13" s="1" t="s">
         <v>76</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>